<commit_message>
create notice and import excel sheet for it
</commit_message>
<xml_diff>
--- a/app/scripts/jobs.xlsx
+++ b/app/scripts/jobs.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
     <sheet name="skills" sheetId="3" r:id="rId2"/>
-    <sheet name="notifications" sheetId="4" r:id="rId3"/>
+    <sheet name="notices" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>No</t>
   </si>
@@ -111,7 +111,7 @@
     <t>breaks wall</t>
   </si>
   <si>
-    <t>Content</t>
+    <t>Contents</t>
   </si>
   <si>
     <t>Type</t>
@@ -123,16 +123,19 @@
     <t>Coming up New Job Item</t>
   </si>
   <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Yes</t>
+    <t>item</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
   <si>
     <t>Fun Competition On New Year 2025</t>
   </si>
   <si>
-    <t>Event</t>
+    <t>event</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -760,9 +763,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1123,20 +1125,20 @@
     <col min="4" max="4" width="10.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1334,20 +1336,20 @@
     <col min="5" max="5" width="11.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1380,7 +1382,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
@@ -1389,16 +1391,16 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1427,7 +1429,7 @@
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>